<commit_message>
Tarea numero 3 completada y subida
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla Automata.xlsx
+++ b/Documentacion/Tabla Automata.xlsx
@@ -722,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,51 +766,117 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -820,15 +886,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -838,65 +895,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,39 +1207,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="F1" s="17" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="F1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="5"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="62" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="7"/>
@@ -1246,25 +1259,25 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="28">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="18" t="s">
         <v>41</v>
       </c>
       <c r="J4" s="1"/>
@@ -1304,7 +1317,7 @@
       <c r="V4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="60"/>
+      <c r="W4" s="45"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="10"/>
@@ -1327,124 +1340,124 @@
       <c r="AQ4" s="11"/>
     </row>
     <row r="5" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="23" t="s">
+      <c r="E5" s="55"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="19" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="52"/>
-      <c r="N5" s="46" t="s">
+      <c r="M5" s="37"/>
+      <c r="N5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="46" t="s">
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="R5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="46" t="s">
+      <c r="S5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="46" t="s">
+      <c r="T5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="53"/>
+      <c r="V5" s="38"/>
     </row>
     <row r="6" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="28">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="28">
         <v>16</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="23" t="s">
+      <c r="E6" s="55"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="19" t="s">
         <v>43</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
-      <c r="V6" s="56"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="41"/>
     </row>
     <row r="7" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="28">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="23" t="s">
+      <c r="E7" s="55"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="54"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="44" t="s">
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
-      <c r="V7" s="56"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="41"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
@@ -1469,19 +1482,19 @@
       <c r="AR7" s="2"/>
     </row>
     <row r="8" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="28">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="23" t="s">
+      <c r="E8" s="55"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="19" t="s">
         <v>45</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1490,34 +1503,34 @@
       <c r="K8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="54"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="43" t="s">
+      <c r="L8" s="39"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="55"/>
-      <c r="V8" s="56"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="41"/>
     </row>
     <row r="9" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="28">
         <v>6</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="28">
         <v>16</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="23" t="s">
+      <c r="E9" s="55"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="19" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1526,106 +1539,106 @@
       <c r="K9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="56"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="41"/>
     </row>
     <row r="10" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="28">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="25" t="s">
+      <c r="E10" s="56"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="20" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="54"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="43" t="s">
+      <c r="L10" s="39"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="55"/>
-      <c r="S10" s="43" t="s">
+      <c r="R10" s="40"/>
+      <c r="S10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="T10" s="55"/>
-      <c r="U10" s="55"/>
-      <c r="V10" s="56"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="41"/>
     </row>
     <row r="11" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="28">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="28">
         <v>16</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="22" t="s">
         <v>50</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="54"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="43" t="s">
+      <c r="L11" s="39"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="V11" s="56"/>
+      <c r="V11" s="41"/>
     </row>
     <row r="12" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="28">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="28" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="25" t="s">
+      <c r="F12" s="49"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="20" t="s">
         <v>51</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1634,206 +1647,206 @@
       <c r="K12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="54"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="43" t="s">
+      <c r="L12" s="39"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="V12" s="48" t="s">
+      <c r="V12" s="33" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:44" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="28">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="28" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="22" t="s">
         <v>53</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="54"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="43" t="s">
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="V13" s="56"/>
+      <c r="V13" s="41"/>
     </row>
     <row r="14" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="28">
         <v>11</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="28">
         <v>16</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="23" t="s">
+      <c r="F14" s="50"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="19" t="s">
         <v>54</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="57"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="49" t="s">
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="V14" s="59"/>
+      <c r="V14" s="44"/>
     </row>
     <row r="15" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="28">
         <v>12</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="28">
         <v>13</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="26" t="s">
         <v>68</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:44" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="28">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="26" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="28">
         <v>14</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="28">
         <v>15</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="22" t="s">
         <v>58</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="28">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="28" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="25" t="s">
+      <c r="F18" s="49"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="20" t="s">
         <v>57</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="28">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="22" t="s">
         <v>60</v>
       </c>
       <c r="J19" s="1"/>
@@ -1843,16 +1856,16 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="22" t="s">
         <v>60</v>
       </c>
       <c r="J20" s="1"/>
@@ -1862,10 +1875,10 @@
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="25" t="s">
+      <c r="E21" s="52"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="20" t="s">
         <v>62</v>
       </c>
       <c r="J21" s="1"/>
@@ -1875,14 +1888,14 @@
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29" t="s">
+      <c r="E22" s="23"/>
+      <c r="F22" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="26" t="s">
         <v>65</v>
       </c>
       <c r="J22" s="1"/>
@@ -1892,16 +1905,16 @@
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="26" t="s">
         <v>65</v>
       </c>
       <c r="J23" s="1"/>
@@ -1912,7 +1925,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="J24" s="1"/>
@@ -2701,6 +2714,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="E4:E10"/>
+    <mergeCell ref="G4:G10"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G17:G18"/>
@@ -2709,13 +2729,6 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="F4:F10"/>
-    <mergeCell ref="E4:E10"/>
-    <mergeCell ref="G4:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>